<commit_message>
Trabajo de hoy terminado, sólo falta lo del tonto inglés
</commit_message>
<xml_diff>
--- a/QiGong/QiGong.xlsx
+++ b/QiGong/QiGong.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elilo\Desktop\Apps\R Studio\Analisis articulo\QiGong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E222D02-53DB-4C01-9FDA-757D27EFA1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FEE009-7F87-4972-8828-A3B3EE6785F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5F071B4E-6846-4105-A160-A2A67249A468}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5F071B4E-6846-4105-A160-A2A67249A468}"/>
   </bookViews>
   <sheets>
     <sheet name="Nback" sheetId="1" r:id="rId1"/>
     <sheet name="Eriksen" sheetId="2" r:id="rId2"/>
-    <sheet name="CFQ" sheetId="3" r:id="rId3"/>
+    <sheet name="DEMO" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,20 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Sj</t>
   </si>
   <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
     <t>2Back_S1_NTg_RC</t>
   </si>
   <si>
@@ -194,6 +185,54 @@
   </si>
   <si>
     <t>S2_TR_Re_FIDI</t>
+  </si>
+  <si>
+    <t>SEXO</t>
+  </si>
+  <si>
+    <t>EDAD</t>
+  </si>
+  <si>
+    <t>CFQ_1</t>
+  </si>
+  <si>
+    <t>CFQ_2</t>
+  </si>
+  <si>
+    <t>IDAREE_1</t>
+  </si>
+  <si>
+    <t>IDARER_1</t>
+  </si>
+  <si>
+    <t>IDEREE_1</t>
+  </si>
+  <si>
+    <t>IDERER_1</t>
+  </si>
+  <si>
+    <t>ACTNO_1</t>
+  </si>
+  <si>
+    <t>ACTFRE_1</t>
+  </si>
+  <si>
+    <t>IDAREE_2</t>
+  </si>
+  <si>
+    <t>IDARER_2</t>
+  </si>
+  <si>
+    <t>IDEREE_2</t>
+  </si>
+  <si>
+    <t>IDERER_2</t>
+  </si>
+  <si>
+    <t>ACTNO_2</t>
+  </si>
+  <si>
+    <t>ACTFRE_2</t>
   </si>
 </sst>
 </file>
@@ -203,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,8 +250,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +296,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -391,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -458,6 +531,25 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,1037 +864,1117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078F59A5-1812-4318-BE45-A03201CEC2B1}">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="H1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="J1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="K1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="L1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="Y1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="Z1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="AA1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="40">
+        <v>2</v>
+      </c>
+      <c r="C2" s="41">
+        <v>52</v>
+      </c>
+      <c r="D2" s="13">
         <v>50.833333333333336</v>
       </c>
-      <c r="C2" s="13">
+      <c r="E2" s="13">
         <v>98.333333333333329</v>
       </c>
-      <c r="D2" s="2">
+      <c r="F2" s="2">
         <v>370.52</v>
       </c>
-      <c r="E2" s="3">
+      <c r="G2" s="3">
         <v>315.51</v>
       </c>
-      <c r="F2" s="13">
+      <c r="H2" s="13">
         <v>76.041666666666671</v>
       </c>
-      <c r="G2" s="13">
+      <c r="I2" s="13">
         <v>58.333333333333336</v>
       </c>
-      <c r="H2" s="13">
+      <c r="J2" s="13">
         <v>85.416666666666671</v>
       </c>
-      <c r="I2" s="13">
+      <c r="K2" s="13">
         <v>87.5</v>
       </c>
-      <c r="J2" s="2">
+      <c r="L2" s="2">
         <v>1.4129366571733726</v>
       </c>
-      <c r="K2" s="2">
+      <c r="M2" s="2">
         <v>2.3006987607520166</v>
       </c>
-      <c r="L2" s="2">
+      <c r="N2" s="2">
         <v>871.67</v>
       </c>
-      <c r="M2" s="2">
+      <c r="O2" s="2">
         <v>733.86</v>
       </c>
-      <c r="N2" s="2">
+      <c r="P2" s="2">
         <v>724.15</v>
       </c>
-      <c r="O2" s="2">
+      <c r="Q2" s="2">
         <v>632.04999999999995</v>
       </c>
-      <c r="P2" s="13">
+      <c r="R2" s="13">
         <v>92.708333333333329</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="S2" s="13">
         <v>33.333333333333336</v>
       </c>
-      <c r="R2" s="13">
+      <c r="T2" s="13">
         <v>83.333333333333329</v>
       </c>
-      <c r="S2" s="13">
+      <c r="U2" s="13">
         <v>62.5</v>
       </c>
-      <c r="T2" s="2">
+      <c r="V2" s="2">
         <v>1.1942534223177415</v>
       </c>
-      <c r="U2" s="2">
+      <c r="W2" s="2">
         <v>1.3286295332139557</v>
       </c>
-      <c r="V2" s="2">
+      <c r="X2" s="2">
         <v>750.76</v>
       </c>
-      <c r="W2" s="2">
+      <c r="Y2" s="2">
         <v>574.75</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Z2" s="2">
         <v>647.11</v>
       </c>
-      <c r="Y2" s="9">
+      <c r="AA2" s="9">
         <v>715.87</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1006</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="40">
+        <v>1</v>
+      </c>
+      <c r="C3" s="41">
+        <v>52</v>
+      </c>
+      <c r="D3" s="13">
         <v>100</v>
       </c>
-      <c r="C3" s="13">
+      <c r="E3" s="13">
         <v>100</v>
       </c>
-      <c r="D3" s="2">
+      <c r="F3" s="2">
         <v>403.94</v>
       </c>
-      <c r="E3" s="3">
+      <c r="G3" s="3">
         <v>408.47</v>
       </c>
-      <c r="F3" s="13">
+      <c r="H3" s="13">
         <v>70.833333333333329</v>
       </c>
-      <c r="G3" s="13">
+      <c r="I3" s="13">
         <v>25</v>
       </c>
-      <c r="H3" s="13">
+      <c r="J3" s="13">
         <v>95.833333333333329</v>
       </c>
-      <c r="I3" s="13">
+      <c r="K3" s="13">
         <v>70.833333333333329</v>
       </c>
-      <c r="J3" s="2">
+      <c r="L3" s="2">
         <v>0.37998270157397107</v>
       </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2">
         <v>1.0970445653961958</v>
       </c>
-      <c r="L3" s="2">
+      <c r="N3" s="2">
         <v>654.82000000000005</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>799</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>681.57</v>
       </c>
-      <c r="O3" s="2">
+      <c r="Q3" s="2">
         <v>857.71</v>
       </c>
-      <c r="P3" s="13">
+      <c r="R3" s="13">
         <v>96.875</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="S3" s="13">
         <v>20.833333333333332</v>
       </c>
-      <c r="R3" s="13">
+      <c r="T3" s="13">
         <v>95.833333333333329</v>
       </c>
-      <c r="S3" s="13">
+      <c r="U3" s="13">
         <v>25</v>
       </c>
-      <c r="T3" s="2">
+      <c r="V3" s="2">
         <v>1.2246163302014752</v>
       </c>
-      <c r="U3" s="2">
+      <c r="W3" s="2">
         <v>1.3623443815053062</v>
       </c>
-      <c r="V3" s="2">
+      <c r="X3" s="2">
         <v>466.15</v>
       </c>
-      <c r="W3" s="2">
+      <c r="Y3" s="2">
         <v>571.20000000000005</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Z3" s="2">
         <v>510.11</v>
       </c>
-      <c r="Y3" s="9">
+      <c r="AA3" s="9">
         <v>776.17</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1008</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="40">
+        <v>2</v>
+      </c>
+      <c r="C4" s="42">
+        <v>54</v>
+      </c>
+      <c r="D4" s="13">
         <v>97.5</v>
       </c>
-      <c r="C4" s="13">
+      <c r="E4" s="13">
         <v>100</v>
       </c>
-      <c r="D4" s="2">
+      <c r="F4" s="2">
         <v>390.55</v>
       </c>
-      <c r="E4" s="3">
+      <c r="G4" s="3">
         <v>371.43</v>
       </c>
-      <c r="F4" s="13">
+      <c r="H4" s="13">
         <v>71.875</v>
       </c>
-      <c r="G4" s="13">
+      <c r="I4" s="13">
         <v>54.166666666666664</v>
       </c>
-      <c r="H4" s="13">
+      <c r="J4" s="13">
         <v>86.458333333333329</v>
       </c>
-      <c r="I4" s="13">
+      <c r="K4" s="13">
         <v>62.5</v>
       </c>
-      <c r="J4" s="2">
+      <c r="L4" s="2">
         <v>1.3627950166771718</v>
       </c>
-      <c r="K4" s="2">
+      <c r="M4" s="2">
         <v>0.7493666632598327</v>
       </c>
-      <c r="L4" s="2">
+      <c r="N4" s="2">
         <v>955.42</v>
       </c>
-      <c r="M4" s="2">
+      <c r="O4" s="2">
         <v>820.31</v>
       </c>
-      <c r="N4" s="2">
+      <c r="P4" s="2">
         <v>795.64</v>
       </c>
-      <c r="O4" s="2">
+      <c r="Q4" s="2">
         <v>928.93</v>
       </c>
-      <c r="P4" s="13">
+      <c r="R4" s="13">
         <v>79.166666666666671</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="S4" s="13">
         <v>54.166666666666664</v>
       </c>
-      <c r="R4" s="13">
+      <c r="T4" s="13">
         <v>90.625</v>
       </c>
-      <c r="S4" s="13">
+      <c r="U4" s="13">
         <v>25</v>
       </c>
-      <c r="T4" s="2">
+      <c r="V4" s="2">
         <v>1.2057789639879286</v>
       </c>
-      <c r="U4" s="2">
+      <c r="W4" s="2">
         <v>0.70850437690455526</v>
       </c>
-      <c r="V4" s="2">
+      <c r="X4" s="2">
         <v>899.07</v>
       </c>
-      <c r="W4" s="2">
+      <c r="Y4" s="2">
         <v>1012.46</v>
       </c>
-      <c r="X4" s="2">
+      <c r="Z4" s="2">
         <v>700.67</v>
       </c>
-      <c r="Y4" s="9">
+      <c r="AA4" s="9">
         <v>935.33</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1009</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="43">
+        <v>2</v>
+      </c>
+      <c r="C5" s="42">
+        <v>59</v>
+      </c>
+      <c r="D5" s="13">
         <v>99.166666666666671</v>
       </c>
-      <c r="C5" s="13">
+      <c r="E5" s="13">
         <v>67.5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" s="2">
         <v>349.83</v>
       </c>
-      <c r="E5" s="3">
+      <c r="G5" s="3">
         <v>415.06</v>
       </c>
-      <c r="F5" s="13">
+      <c r="H5" s="13">
         <v>88.541666666666671</v>
       </c>
-      <c r="G5" s="13">
+      <c r="I5" s="13">
         <v>70.833333333333329</v>
       </c>
-      <c r="H5" s="13">
+      <c r="J5" s="13">
         <v>80.208333333333329</v>
       </c>
-      <c r="I5" s="13">
+      <c r="K5" s="13">
         <v>75</v>
       </c>
-      <c r="J5" s="2">
+      <c r="L5" s="2">
         <v>1.8665331800016349</v>
       </c>
-      <c r="K5" s="2">
+      <c r="M5" s="2">
         <v>1.4867075516959951</v>
       </c>
-      <c r="L5" s="2">
+      <c r="N5" s="2">
         <v>871.36</v>
       </c>
-      <c r="M5" s="2">
+      <c r="O5" s="2">
         <v>904.12</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>867.34</v>
       </c>
-      <c r="O5" s="2">
+      <c r="Q5" s="2">
         <v>728.44</v>
       </c>
-      <c r="P5" s="13">
+      <c r="R5" s="13">
         <v>78.125</v>
-      </c>
-      <c r="Q5" s="13">
-        <v>33.333333333333336</v>
-      </c>
-      <c r="R5" s="13">
-        <v>65.625</v>
       </c>
       <c r="S5" s="13">
         <v>33.333333333333336</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="13">
+        <v>65.625</v>
+      </c>
+      <c r="U5" s="13">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="V5" s="2">
         <v>0.82743426176763901</v>
       </c>
-      <c r="U5" s="2">
+      <c r="W5" s="2">
         <v>0.82743426176763901</v>
       </c>
-      <c r="V5" s="2">
+      <c r="X5" s="2">
         <v>841.79</v>
       </c>
-      <c r="W5" s="2">
+      <c r="Y5" s="2">
         <v>810.5</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Z5" s="2">
         <v>832.21</v>
       </c>
-      <c r="Y5" s="9">
+      <c r="AA5" s="9">
         <v>722.88</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1010</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="40">
+        <v>2</v>
+      </c>
+      <c r="C6" s="42">
+        <v>53</v>
+      </c>
+      <c r="D6" s="13">
         <v>99.166666666666671</v>
       </c>
-      <c r="C6" s="13">
+      <c r="E6" s="13">
         <v>99.166666666666671</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F6" s="2">
         <v>359.06</v>
       </c>
-      <c r="E6" s="3">
+      <c r="G6" s="3">
         <v>320.52999999999997</v>
       </c>
-      <c r="F6" s="13">
+      <c r="H6" s="13">
         <v>78.125</v>
       </c>
-      <c r="G6" s="13">
+      <c r="I6" s="13">
         <v>75</v>
       </c>
-      <c r="H6" s="13">
+      <c r="J6" s="13">
         <v>61.458333333333336</v>
       </c>
-      <c r="I6" s="13">
+      <c r="K6" s="13">
         <v>79.166666666666671</v>
       </c>
-      <c r="J6" s="2">
+      <c r="L6" s="2">
         <v>1.5616363092149581</v>
       </c>
-      <c r="K6" s="2">
+      <c r="M6" s="2">
         <v>1.6244356029998261</v>
       </c>
-      <c r="L6" s="2">
+      <c r="N6" s="2">
         <v>731.29</v>
       </c>
-      <c r="M6" s="2">
+      <c r="O6" s="2">
         <v>685.06</v>
       </c>
-      <c r="N6" s="2">
+      <c r="P6" s="2">
         <v>983.15</v>
       </c>
-      <c r="O6" s="2">
+      <c r="Q6" s="2">
         <v>778.26</v>
       </c>
-      <c r="P6" s="13">
+      <c r="R6" s="13">
         <v>50</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="S6" s="13">
         <v>33.333333333333336</v>
       </c>
-      <c r="R6" s="13">
+      <c r="T6" s="13">
         <v>39.583333333333336</v>
       </c>
-      <c r="S6" s="13">
+      <c r="U6" s="13">
         <v>37.5</v>
       </c>
-      <c r="T6" s="2">
+      <c r="V6" s="2">
         <v>-0.22029890504753266</v>
       </c>
-      <c r="U6" s="2">
+      <c r="W6" s="2">
         <v>-0.42327281957845042</v>
       </c>
-      <c r="V6" s="2">
+      <c r="X6" s="2">
         <v>696.35</v>
       </c>
-      <c r="W6" s="2">
+      <c r="Y6" s="2">
         <v>609.75</v>
       </c>
-      <c r="X6" s="2">
+      <c r="Z6" s="2">
         <v>659.5</v>
       </c>
-      <c r="Y6" s="9">
+      <c r="AA6" s="9">
         <v>663.44</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1012</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="40">
+        <v>2</v>
+      </c>
+      <c r="C7" s="42">
+        <v>64</v>
+      </c>
+      <c r="D7" s="13">
         <v>85</v>
       </c>
-      <c r="C7" s="13">
+      <c r="E7" s="13">
         <v>99.166666666666671</v>
       </c>
-      <c r="D7" s="2">
+      <c r="F7" s="2">
         <v>319.08999999999997</v>
       </c>
-      <c r="E7" s="3">
+      <c r="G7" s="3">
         <v>299.94</v>
       </c>
-      <c r="F7" s="13">
+      <c r="H7" s="13">
         <v>12.5</v>
       </c>
-      <c r="G7" s="13">
+      <c r="I7" s="13">
         <v>79.166666666666671</v>
       </c>
-      <c r="H7" s="13">
+      <c r="J7" s="13">
         <v>43.75</v>
       </c>
-      <c r="I7" s="13">
+      <c r="K7" s="13">
         <v>66.666666666666671</v>
       </c>
-      <c r="J7" s="2">
+      <c r="L7" s="2">
         <v>0.46598353790003089</v>
       </c>
-      <c r="K7" s="2">
+      <c r="M7" s="2">
         <v>0.97924958199355561</v>
       </c>
-      <c r="L7" s="2">
+      <c r="N7" s="2">
         <v>884.25</v>
       </c>
-      <c r="M7" s="2">
+      <c r="O7" s="2">
         <v>835.16</v>
       </c>
-      <c r="N7" s="2">
+      <c r="P7" s="2">
         <v>668.45</v>
       </c>
-      <c r="O7" s="2">
+      <c r="Q7" s="2">
         <v>603.94000000000005</v>
       </c>
-      <c r="P7" s="13">
+      <c r="R7" s="13">
         <v>26.041666666666668</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="S7" s="13">
         <v>62.5</v>
       </c>
-      <c r="R7" s="13">
+      <c r="T7" s="13">
         <v>37.5</v>
       </c>
-      <c r="S7" s="13">
+      <c r="U7" s="13">
         <v>87.5</v>
       </c>
-      <c r="T7" s="2">
+      <c r="V7" s="2">
         <v>-0.11208793533108252</v>
       </c>
-      <c r="U7" s="2">
+      <c r="W7" s="2">
         <v>0.83171001641163311</v>
       </c>
-      <c r="V7" s="2">
+      <c r="X7" s="2">
         <v>982</v>
       </c>
-      <c r="W7" s="2">
+      <c r="Y7" s="2">
         <v>858.6</v>
       </c>
-      <c r="X7" s="2">
+      <c r="Z7" s="2">
         <v>612.66999999999996</v>
       </c>
-      <c r="Y7" s="9">
+      <c r="AA7" s="9">
         <v>577.80999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1017</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="40">
+        <v>2</v>
+      </c>
+      <c r="C8" s="41">
+        <v>51</v>
+      </c>
+      <c r="D8" s="13">
         <v>94.166666666666671</v>
       </c>
-      <c r="C8" s="13">
+      <c r="E8" s="13">
         <v>99.166666666666671</v>
       </c>
-      <c r="D8" s="2">
+      <c r="F8" s="2">
         <v>345.04</v>
       </c>
-      <c r="E8" s="3">
+      <c r="G8" s="3">
         <v>317.66000000000003</v>
       </c>
-      <c r="F8" s="13">
+      <c r="H8" s="13">
         <v>73.958333333333329</v>
       </c>
-      <c r="G8" s="13">
+      <c r="I8" s="13">
         <v>75</v>
       </c>
-      <c r="H8" s="13">
+      <c r="J8" s="13">
         <v>47.916666666666664</v>
       </c>
-      <c r="I8" s="13">
+      <c r="K8" s="13">
         <v>62.5</v>
       </c>
-      <c r="J8" s="2">
+      <c r="L8" s="2">
         <v>1.6844799194456623</v>
       </c>
-      <c r="K8" s="2">
+      <c r="M8" s="2">
         <v>0.86716164666247308</v>
       </c>
-      <c r="L8" s="2">
+      <c r="N8" s="2">
         <v>752.69</v>
       </c>
-      <c r="M8" s="2">
+      <c r="O8" s="2">
         <v>720.5</v>
       </c>
-      <c r="N8" s="2">
+      <c r="P8" s="2">
         <v>689.04</v>
       </c>
-      <c r="O8" s="2">
+      <c r="Q8" s="2">
         <v>709.53</v>
       </c>
-      <c r="P8" s="13">
+      <c r="R8" s="13">
         <v>81.25</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="S8" s="13">
         <v>33.333333333333336</v>
       </c>
-      <c r="R8" s="13">
+      <c r="T8" s="13">
         <v>58.333333333333336</v>
       </c>
-      <c r="S8" s="13">
+      <c r="U8" s="13">
         <v>29.166666666666668</v>
       </c>
-      <c r="T8" s="2">
+      <c r="V8" s="2">
         <v>0.88728359800807965</v>
       </c>
-      <c r="U8" s="2">
+      <c r="W8" s="2">
         <v>-0.11779498340264039</v>
       </c>
-      <c r="V8" s="2">
+      <c r="X8" s="2">
         <v>457.27</v>
       </c>
-      <c r="W8" s="2">
+      <c r="Y8" s="2">
         <v>633.88</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Z8" s="2">
         <v>672.34</v>
       </c>
-      <c r="Y8" s="9">
+      <c r="AA8" s="9">
         <v>896.29</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1020</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="44">
+        <v>2</v>
+      </c>
+      <c r="C9" s="40">
+        <v>31</v>
+      </c>
+      <c r="D9" s="13">
         <v>99.166666666666671</v>
       </c>
-      <c r="C9" s="13">
+      <c r="E9" s="13">
         <v>100</v>
       </c>
-      <c r="D9" s="2">
+      <c r="F9" s="2">
         <v>328.08</v>
       </c>
-      <c r="E9" s="3">
+      <c r="G9" s="3">
         <v>370.73</v>
       </c>
-      <c r="F9" s="13">
+      <c r="H9" s="13">
         <v>90.625</v>
-      </c>
-      <c r="G9" s="13">
-        <v>83.333333333333329</v>
-      </c>
-      <c r="H9" s="13">
-        <v>94.791666666666671</v>
       </c>
       <c r="I9" s="13">
         <v>83.333333333333329</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="13">
+        <v>94.791666666666671</v>
+      </c>
+      <c r="K9" s="13">
+        <v>83.333333333333329</v>
+      </c>
+      <c r="L9" s="2">
         <v>2.5924022877148993</v>
       </c>
-      <c r="K9" s="2">
+      <c r="M9" s="2">
         <v>1.9348431322034023</v>
       </c>
-      <c r="L9" s="2">
+      <c r="N9" s="2">
         <v>767.21</v>
       </c>
-      <c r="M9" s="2">
+      <c r="O9" s="2">
         <v>728.55</v>
       </c>
-      <c r="N9" s="2">
+      <c r="P9" s="2">
         <v>626.54</v>
       </c>
-      <c r="O9" s="2">
+      <c r="Q9" s="2">
         <v>557.35</v>
       </c>
-      <c r="P9" s="13">
+      <c r="R9" s="13">
         <v>79.166666666666671</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="S9" s="13">
         <v>70.833333333333329</v>
       </c>
-      <c r="R9" s="13">
+      <c r="T9" s="13">
         <v>90.625</v>
       </c>
-      <c r="S9" s="13">
+      <c r="U9" s="13">
         <v>66.666666666666671</v>
       </c>
-      <c r="T9" s="2">
+      <c r="V9" s="2">
         <v>1.8066838437611943</v>
       </c>
-      <c r="U9" s="2">
+      <c r="W9" s="2">
         <v>1.7487381965989948</v>
       </c>
-      <c r="V9" s="2">
+      <c r="X9" s="2">
         <v>821.91</v>
       </c>
-      <c r="W9" s="2">
+      <c r="Y9" s="2">
         <v>849.82</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Z9" s="2">
         <v>630.89</v>
       </c>
-      <c r="Y9" s="9">
+      <c r="AA9" s="9">
         <v>558.80999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1021</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="45">
+        <v>2</v>
+      </c>
+      <c r="C10" s="45">
+        <v>40</v>
+      </c>
+      <c r="D10" s="13">
         <v>99.166666666666671</v>
       </c>
-      <c r="C10" s="13">
+      <c r="E10" s="13">
         <v>100</v>
       </c>
-      <c r="D10" s="2">
+      <c r="F10" s="2">
         <v>300.73</v>
       </c>
-      <c r="E10" s="3">
+      <c r="G10" s="3">
         <v>320.27</v>
       </c>
-      <c r="F10" s="13">
+      <c r="H10" s="13">
         <v>78.125</v>
       </c>
-      <c r="G10" s="13">
+      <c r="I10" s="13">
         <v>20.833333333333332</v>
       </c>
-      <c r="H10" s="13">
+      <c r="J10" s="13">
         <v>42.708333333333336</v>
       </c>
-      <c r="I10" s="13">
+      <c r="K10" s="13">
         <v>41.666666666666664</v>
       </c>
-      <c r="J10" s="2">
+      <c r="L10" s="2">
         <v>-3.5796040351985137E-2</v>
       </c>
-      <c r="K10" s="2">
+      <c r="M10" s="2">
         <v>0.10821096971645036</v>
       </c>
-      <c r="L10" s="2">
+      <c r="N10" s="2">
         <v>523.32000000000005</v>
       </c>
-      <c r="M10" s="2">
+      <c r="O10" s="2">
         <v>637.4</v>
       </c>
-      <c r="N10" s="2">
+      <c r="P10" s="2">
         <v>567.04999999999995</v>
       </c>
-      <c r="O10" s="2">
+      <c r="Q10" s="2">
         <v>451.8</v>
       </c>
-      <c r="P10" s="13">
+      <c r="R10" s="13">
         <v>72.916666666666671</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="S10" s="13">
         <v>12.5</v>
       </c>
-      <c r="R10" s="13">
+      <c r="T10" s="13">
         <v>45.833333333333336</v>
       </c>
-      <c r="S10" s="13">
+      <c r="U10" s="13">
         <v>20.833333333333332</v>
       </c>
-      <c r="T10" s="2">
+      <c r="V10" s="2">
         <v>-0.26320282135713224</v>
       </c>
-      <c r="U10" s="2">
+      <c r="W10" s="2">
         <v>-0.70758434588583785</v>
       </c>
-      <c r="V10" s="2">
+      <c r="X10" s="2">
         <v>512.97</v>
       </c>
-      <c r="W10" s="2">
+      <c r="Y10" s="2">
         <v>836.33</v>
       </c>
-      <c r="X10" s="2">
+      <c r="Z10" s="2">
         <v>477.25</v>
       </c>
-      <c r="Y10" s="9">
+      <c r="AA10" s="9">
         <v>496.8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1023</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="40">
+        <v>1</v>
+      </c>
+      <c r="C11" s="40">
+        <v>33</v>
+      </c>
+      <c r="D11" s="13">
         <v>99.166666666666671</v>
       </c>
-      <c r="C11" s="13">
+      <c r="E11" s="13">
         <v>87.5</v>
       </c>
-      <c r="D11" s="2">
+      <c r="F11" s="2">
         <v>293.16000000000003</v>
       </c>
-      <c r="E11" s="3">
+      <c r="G11" s="3">
         <v>313.39</v>
       </c>
-      <c r="F11" s="13">
+      <c r="H11" s="13">
         <v>87.5</v>
       </c>
-      <c r="G11" s="13">
+      <c r="I11" s="13">
         <v>79.166666666666671</v>
       </c>
-      <c r="H11" s="13">
+      <c r="J11" s="13">
         <v>96.875</v>
       </c>
-      <c r="I11" s="13">
+      <c r="K11" s="13">
         <v>70.833333333333329</v>
       </c>
-      <c r="J11" s="2">
+      <c r="L11" s="2">
         <v>2.0147260644253611</v>
       </c>
-      <c r="K11" s="2">
+      <c r="M11" s="2">
         <v>1.5159438487997996</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N11" s="2">
         <v>703.65</v>
       </c>
-      <c r="M11" s="2">
+      <c r="O11" s="2">
         <v>638.26</v>
       </c>
-      <c r="N11" s="2">
+      <c r="P11" s="2">
         <v>562.26</v>
       </c>
-      <c r="O11" s="2">
+      <c r="Q11" s="2">
         <v>559.41</v>
       </c>
-      <c r="P11" s="13">
+      <c r="R11" s="13">
         <v>83.333333333333329</v>
-      </c>
-      <c r="Q11" s="13">
-        <v>33.333333333333336</v>
-      </c>
-      <c r="R11" s="13">
-        <v>85.416666666666671</v>
       </c>
       <c r="S11" s="13">
         <v>33.333333333333336</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="13">
+        <v>85.416666666666671</v>
+      </c>
+      <c r="U11" s="13">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="V11" s="2">
         <v>0.95226682780517968</v>
       </c>
-      <c r="U11" s="2">
+      <c r="W11" s="2">
         <v>1.023680303560583</v>
       </c>
-      <c r="V11" s="2">
+      <c r="X11" s="2">
         <v>711.9</v>
       </c>
-      <c r="W11" s="2">
+      <c r="Y11" s="2">
         <v>595.63</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Z11" s="2">
         <v>649.54999999999995</v>
       </c>
-      <c r="Y11" s="9">
+      <c r="AA11" s="9">
         <v>572.38</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1024</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="40">
+        <v>2</v>
+      </c>
+      <c r="C12" s="40">
+        <v>49</v>
+      </c>
+      <c r="D12" s="13">
         <v>100</v>
       </c>
-      <c r="C12" s="13">
+      <c r="E12" s="13">
         <v>100</v>
       </c>
-      <c r="D12" s="2">
+      <c r="F12" s="2">
         <v>347.04</v>
       </c>
-      <c r="E12" s="3">
+      <c r="G12" s="3">
         <v>332.38</v>
       </c>
-      <c r="F12" s="13">
+      <c r="H12" s="13">
         <v>71.875</v>
       </c>
-      <c r="G12" s="13">
+      <c r="I12" s="13">
         <v>54.166666666666664</v>
       </c>
-      <c r="H12" s="13">
+      <c r="J12" s="13">
         <v>96.875</v>
       </c>
-      <c r="I12" s="13">
+      <c r="K12" s="13">
         <v>83.333333333333329</v>
       </c>
-      <c r="J12" s="2">
+      <c r="L12" s="2">
         <v>0.88105521676200316</v>
       </c>
-      <c r="K12" s="2">
+      <c r="M12" s="2">
         <v>2.3504156932023377</v>
       </c>
-      <c r="L12" s="2">
+      <c r="N12" s="2">
         <v>851.2</v>
       </c>
-      <c r="M12" s="2">
+      <c r="O12" s="2">
         <v>746</v>
       </c>
-      <c r="N12" s="2">
+      <c r="P12" s="2">
         <v>647.86</v>
       </c>
-      <c r="O12" s="2">
+      <c r="Q12" s="2">
         <v>759.15</v>
       </c>
-      <c r="P12" s="13">
+      <c r="R12" s="13">
         <v>52.083333333333336</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="S12" s="13">
         <v>29.166666666666668</v>
       </c>
-      <c r="R12" s="13">
+      <c r="T12" s="13">
         <v>85.416666666666671</v>
       </c>
-      <c r="S12" s="13">
+      <c r="U12" s="13">
         <v>70.833333333333329</v>
       </c>
-      <c r="T12" s="2">
+      <c r="V12" s="2">
         <v>0.46146788655148263</v>
       </c>
-      <c r="U12" s="2">
+      <c r="W12" s="2">
         <v>1.9315164097987352</v>
       </c>
-      <c r="V12" s="2">
+      <c r="X12" s="2">
         <v>826.44</v>
       </c>
-      <c r="W12" s="2">
+      <c r="Y12" s="2">
         <v>697.71</v>
       </c>
-      <c r="X12" s="2">
+      <c r="Z12" s="2">
         <v>741.55</v>
       </c>
-      <c r="Y12" s="9">
+      <c r="AA12" s="9">
         <v>700.88</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1025</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="40">
+        <v>2</v>
+      </c>
+      <c r="C13" s="40">
+        <v>52</v>
+      </c>
+      <c r="D13" s="14">
         <v>100</v>
       </c>
-      <c r="C13" s="14">
+      <c r="E13" s="14">
         <v>99.166666666666671</v>
       </c>
-      <c r="D13" s="4">
+      <c r="F13" s="4">
         <v>349.42</v>
       </c>
-      <c r="E13" s="5">
+      <c r="G13" s="5">
         <v>382.72</v>
       </c>
-      <c r="F13" s="16">
+      <c r="H13" s="16">
         <v>58.333333333333336</v>
-      </c>
-      <c r="G13" s="16">
-        <v>37.5</v>
-      </c>
-      <c r="H13" s="16">
-        <v>68.75</v>
       </c>
       <c r="I13" s="16">
         <v>37.5</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="16">
+        <v>68.75</v>
+      </c>
+      <c r="K13" s="16">
+        <v>37.5</v>
+      </c>
+      <c r="L13" s="8">
         <v>0.26049279829118066</v>
       </c>
-      <c r="K13" s="8">
+      <c r="M13" s="8">
         <v>-0.52906775821230001</v>
       </c>
-      <c r="L13" s="8">
+      <c r="N13" s="8">
         <v>595.21</v>
       </c>
-      <c r="M13" s="8">
+      <c r="O13" s="8">
         <v>726.44</v>
       </c>
-      <c r="N13" s="8">
+      <c r="P13" s="8">
         <v>501.02</v>
       </c>
-      <c r="O13" s="8">
+      <c r="Q13" s="8">
         <v>411.44</v>
       </c>
-      <c r="P13" s="17">
+      <c r="R13" s="17">
         <v>55.208333333333336</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="S13" s="17">
         <v>37.5</v>
       </c>
-      <c r="R13" s="17">
+      <c r="T13" s="17">
         <v>60.416666666666664</v>
       </c>
-      <c r="S13" s="17">
+      <c r="U13" s="17">
         <v>20.833333333333332</v>
       </c>
-      <c r="T13" s="10">
+      <c r="V13" s="10">
         <v>-2.7354330960974227E-2</v>
       </c>
-      <c r="U13" s="10">
+      <c r="W13" s="10">
         <v>-0.46598353790003078</v>
       </c>
-      <c r="V13" s="10">
+      <c r="X13" s="10">
         <v>545.91</v>
       </c>
-      <c r="W13" s="10">
+      <c r="Y13" s="10">
         <v>679.67</v>
       </c>
-      <c r="X13" s="10">
+      <c r="Z13" s="10">
         <v>496.17</v>
       </c>
-      <c r="Y13" s="11">
+      <c r="AA13" s="11">
         <v>624</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1814,7 +1986,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1851,76 +2023,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="F1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="G1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="H1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="I1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="J1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="K1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="L1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="M1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="N1" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="O1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="P1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="Q1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="R1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="S1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="T1" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="U1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="V1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="24" t="s">
+      <c r="W1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="X1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="Y1" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -3175,188 +3347,877 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BDFCEE-E37A-4100-8FA8-7ECA83C0B023}">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C43D779-65E3-4EC4-ADC7-F39789FCF075}">
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="38">
+        <v>1001</v>
+      </c>
+      <c r="B2" s="38">
+        <v>2</v>
+      </c>
+      <c r="C2" s="38">
+        <v>52</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>41</v>
+      </c>
+      <c r="F2">
+        <v>48</v>
+      </c>
+      <c r="G2">
+        <v>47</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+      <c r="I2">
+        <v>80</v>
+      </c>
+      <c r="J2">
+        <v>52</v>
+      </c>
+      <c r="K2">
+        <v>43</v>
+      </c>
+      <c r="L2">
+        <v>44</v>
+      </c>
+      <c r="M2">
+        <v>45</v>
+      </c>
+      <c r="N2">
+        <v>11</v>
+      </c>
+      <c r="O2">
+        <v>67</v>
+      </c>
+      <c r="P2">
+        <v>31</v>
+      </c>
+      <c r="Q2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="38">
+        <v>1006</v>
+      </c>
+      <c r="B3" s="38">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" s="38">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>48</v>
+      </c>
+      <c r="E3">
+        <v>46</v>
+      </c>
+      <c r="F3">
+        <v>43</v>
+      </c>
+      <c r="G3">
+        <v>42</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <v>74</v>
+      </c>
+      <c r="J3">
+        <v>48</v>
+      </c>
+      <c r="K3">
+        <v>43</v>
+      </c>
+      <c r="L3">
+        <v>38</v>
+      </c>
+      <c r="M3">
+        <v>47</v>
+      </c>
+      <c r="N3">
+        <v>15</v>
+      </c>
+      <c r="O3">
+        <v>77</v>
+      </c>
+      <c r="P3">
+        <v>28</v>
+      </c>
+      <c r="Q3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="38">
+        <v>1008</v>
+      </c>
+      <c r="B4" s="38">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1001</v>
-      </c>
-      <c r="B2">
+      <c r="C4" s="38">
+        <v>54</v>
+      </c>
+      <c r="D4">
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>49</v>
+      </c>
+      <c r="G4">
+        <v>46</v>
+      </c>
+      <c r="H4">
+        <v>11</v>
+      </c>
+      <c r="I4">
+        <v>115</v>
+      </c>
+      <c r="J4">
+        <v>47</v>
+      </c>
+      <c r="K4">
+        <v>45</v>
+      </c>
+      <c r="L4">
+        <v>43</v>
+      </c>
+      <c r="M4">
+        <v>42</v>
+      </c>
+      <c r="N4">
+        <v>11</v>
+      </c>
+      <c r="O4">
+        <v>86</v>
+      </c>
+      <c r="P4">
+        <v>34</v>
+      </c>
+      <c r="Q4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="38">
+        <v>1009</v>
+      </c>
+      <c r="B5" s="46">
+        <v>2</v>
+      </c>
+      <c r="C5" s="38">
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <v>42</v>
+      </c>
+      <c r="E5">
+        <v>34</v>
+      </c>
+      <c r="F5">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <v>33</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>94</v>
+      </c>
+      <c r="J5">
+        <v>43</v>
+      </c>
+      <c r="K5">
+        <v>37</v>
+      </c>
+      <c r="L5">
+        <v>37</v>
+      </c>
+      <c r="M5">
+        <v>37</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="O5">
+        <v>97</v>
+      </c>
+      <c r="P5">
+        <v>40</v>
+      </c>
+      <c r="Q5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="38">
+        <v>1010</v>
+      </c>
+      <c r="B6" s="38">
+        <v>2</v>
+      </c>
+      <c r="C6" s="38">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>54</v>
+      </c>
+      <c r="E6">
+        <v>43</v>
+      </c>
+      <c r="F6">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>41</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>65.5</v>
+      </c>
+      <c r="J6">
+        <v>43</v>
+      </c>
+      <c r="K6">
+        <v>46</v>
+      </c>
+      <c r="L6">
+        <v>41</v>
+      </c>
+      <c r="M6">
+        <v>45</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <v>47</v>
+      </c>
+      <c r="P6">
+        <v>20</v>
+      </c>
+      <c r="Q6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="38">
+        <v>1011</v>
+      </c>
+      <c r="B7" s="38">
+        <v>1</v>
+      </c>
+      <c r="C7" s="38">
+        <v>43</v>
+      </c>
+      <c r="D7">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>44</v>
+      </c>
+      <c r="G7">
+        <v>43</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>62</v>
+      </c>
+      <c r="J7">
+        <v>36</v>
+      </c>
+      <c r="K7">
+        <v>37</v>
+      </c>
+      <c r="L7">
+        <v>45</v>
+      </c>
+      <c r="M7">
+        <v>39</v>
+      </c>
+      <c r="N7">
+        <v>12</v>
+      </c>
+      <c r="O7">
+        <v>156</v>
+      </c>
+      <c r="P7">
+        <v>19</v>
+      </c>
+      <c r="Q7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="38">
+        <v>1012</v>
+      </c>
+      <c r="B8" s="38">
+        <v>2</v>
+      </c>
+      <c r="C8" s="38">
+        <v>64</v>
+      </c>
+      <c r="D8">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>44</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>45</v>
+      </c>
+      <c r="K8">
+        <v>47</v>
+      </c>
+      <c r="L8">
+        <v>40</v>
+      </c>
+      <c r="M8">
+        <v>42</v>
+      </c>
+      <c r="N8">
+        <v>8</v>
+      </c>
+      <c r="O8">
+        <v>113</v>
+      </c>
+      <c r="P8">
+        <v>27</v>
+      </c>
+      <c r="Q8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="38">
+        <v>1014</v>
+      </c>
+      <c r="B9" s="38">
+        <v>2</v>
+      </c>
+      <c r="C9" s="38">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>43</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
+      </c>
+      <c r="G9">
+        <v>36</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>48</v>
+      </c>
+      <c r="K9">
+        <v>46</v>
+      </c>
+      <c r="L9">
+        <v>48</v>
+      </c>
+      <c r="M9">
+        <v>45</v>
+      </c>
+      <c r="N9">
+        <v>9</v>
+      </c>
+      <c r="O9">
+        <v>83</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="38">
+        <v>1017</v>
+      </c>
+      <c r="B10" s="38">
+        <v>2</v>
+      </c>
+      <c r="C10" s="38">
+        <v>51</v>
+      </c>
+      <c r="D10">
+        <v>44</v>
+      </c>
+      <c r="E10">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>42</v>
+      </c>
+      <c r="G10">
+        <v>46</v>
+      </c>
+      <c r="H10">
+        <v>11</v>
+      </c>
+      <c r="I10">
+        <v>128</v>
+      </c>
+      <c r="J10">
+        <v>41</v>
+      </c>
+      <c r="K10">
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <v>41</v>
+      </c>
+      <c r="M10">
+        <v>48</v>
+      </c>
+      <c r="N10">
+        <v>11</v>
+      </c>
+      <c r="O10">
+        <v>151</v>
+      </c>
+      <c r="P10">
+        <v>27</v>
+      </c>
+      <c r="Q10">
         <v>31</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>1019</v>
+      </c>
+      <c r="B11" s="46">
+        <v>2</v>
+      </c>
+      <c r="C11" s="38">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>46</v>
+      </c>
+      <c r="F11">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1006</v>
-      </c>
-      <c r="B3">
-        <v>28</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>1008</v>
-      </c>
-      <c r="B4">
+      <c r="G11">
+        <v>47</v>
+      </c>
+      <c r="H11">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>89</v>
+      </c>
+      <c r="J11">
+        <v>48</v>
+      </c>
+      <c r="K11">
+        <v>46</v>
+      </c>
+      <c r="L11">
+        <v>42</v>
+      </c>
+      <c r="M11">
+        <v>46</v>
+      </c>
+      <c r="N11">
+        <v>13</v>
+      </c>
+      <c r="O11">
+        <v>134</v>
+      </c>
+      <c r="P11">
+        <v>31</v>
+      </c>
+      <c r="Q11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>1020</v>
+      </c>
+      <c r="B12" s="46">
+        <v>2</v>
+      </c>
+      <c r="C12" s="38">
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <v>47</v>
+      </c>
+      <c r="E12">
+        <v>54</v>
+      </c>
+      <c r="F12">
+        <v>38</v>
+      </c>
+      <c r="G12">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
         <v>34</v>
       </c>
-      <c r="C4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1009</v>
-      </c>
-      <c r="B5">
+      <c r="J12">
+        <v>41</v>
+      </c>
+      <c r="K12">
+        <v>56</v>
+      </c>
+      <c r="L12">
+        <v>52</v>
+      </c>
+      <c r="M12">
+        <v>52</v>
+      </c>
+      <c r="N12">
+        <v>8</v>
+      </c>
+      <c r="O12">
+        <v>24</v>
+      </c>
+      <c r="P12">
+        <v>42</v>
+      </c>
+      <c r="Q12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="38">
+        <v>1021</v>
+      </c>
+      <c r="B13" s="38">
+        <v>2</v>
+      </c>
+      <c r="C13" s="38">
         <v>40</v>
       </c>
-      <c r="C5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1010</v>
-      </c>
-      <c r="B6">
+      <c r="D13">
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="G13">
+        <v>42</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>42</v>
+      </c>
+      <c r="J13">
+        <v>39</v>
+      </c>
+      <c r="K13">
+        <v>42</v>
+      </c>
+      <c r="L13">
+        <v>42</v>
+      </c>
+      <c r="M13">
+        <v>43</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="O13">
+        <v>34</v>
+      </c>
+      <c r="P13">
+        <v>36</v>
+      </c>
+      <c r="Q13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="38">
+        <v>1023</v>
+      </c>
+      <c r="B14" s="38">
+        <v>1</v>
+      </c>
+      <c r="C14" s="38">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>48</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="F14">
+        <v>43</v>
+      </c>
+      <c r="G14">
+        <v>51</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>130</v>
+      </c>
+      <c r="J14">
+        <v>46</v>
+      </c>
+      <c r="K14">
+        <v>46</v>
+      </c>
+      <c r="L14">
+        <v>54</v>
+      </c>
+      <c r="M14">
+        <v>51</v>
+      </c>
+      <c r="N14">
         <v>20</v>
       </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>1011</v>
-      </c>
-      <c r="B7">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>1012</v>
-      </c>
-      <c r="B8">
+      <c r="O14">
+        <v>167</v>
+      </c>
+      <c r="P14">
         <v>27</v>
       </c>
-      <c r="C8">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>1014</v>
-      </c>
-      <c r="B9">
+      <c r="Q14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="38">
+        <v>1024</v>
+      </c>
+      <c r="B15" s="38">
+        <v>2</v>
+      </c>
+      <c r="C15" s="38">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>36</v>
+      </c>
+      <c r="E15">
+        <v>39</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+      <c r="G15">
+        <v>39</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>38</v>
+      </c>
+      <c r="J15">
+        <v>44</v>
+      </c>
+      <c r="K15">
+        <v>39</v>
+      </c>
+      <c r="L15">
+        <v>42</v>
+      </c>
+      <c r="M15">
+        <v>36</v>
+      </c>
+      <c r="N15">
+        <v>7</v>
+      </c>
+      <c r="O15">
+        <v>38</v>
+      </c>
+      <c r="P15">
+        <v>27</v>
+      </c>
+      <c r="Q15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="38">
+        <v>1025</v>
+      </c>
+      <c r="B16" s="38">
+        <v>2</v>
+      </c>
+      <c r="C16" s="38">
+        <v>52</v>
+      </c>
+      <c r="D16">
+        <v>38</v>
+      </c>
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16">
+        <v>45</v>
+      </c>
+      <c r="G16">
+        <v>46</v>
+      </c>
+      <c r="H16">
         <v>10</v>
       </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1017</v>
-      </c>
-      <c r="B10">
-        <v>27</v>
-      </c>
-      <c r="C10">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1019</v>
-      </c>
-      <c r="B11">
-        <v>31</v>
-      </c>
-      <c r="C11">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1020</v>
-      </c>
-      <c r="B12">
+      <c r="I16">
+        <v>43</v>
+      </c>
+      <c r="J16">
+        <v>53</v>
+      </c>
+      <c r="K16">
+        <v>43</v>
+      </c>
+      <c r="L16">
         <v>42</v>
       </c>
-      <c r="C12">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1021</v>
-      </c>
-      <c r="B13">
-        <v>36</v>
-      </c>
-      <c r="C13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1023</v>
-      </c>
-      <c r="B14">
-        <v>27</v>
-      </c>
-      <c r="C14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1024</v>
-      </c>
-      <c r="B15">
-        <v>27</v>
-      </c>
-      <c r="C15">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1025</v>
-      </c>
-      <c r="B16">
+      <c r="M16">
+        <v>45</v>
+      </c>
+      <c r="N16">
+        <v>12</v>
+      </c>
+      <c r="O16">
+        <v>56</v>
+      </c>
+      <c r="P16">
         <v>33</v>
       </c>
-      <c r="C16">
+      <c r="Q16">
         <v>35</v>
       </c>
     </row>

</xml_diff>